<commit_message>
[Improvement] On terminology : babies_potential -> babies_service ; on readme
</commit_message>
<xml_diff>
--- a/scenarios/exemple/input_exemple.xlsx
+++ b/scenarios/exemple/input_exemple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS5997\src\neonat\scenarios\exemple\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684502BF-6F6D-4607-B274-E15E69317F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C398C0-EBF0-43D7-B951-C2698F36A864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="babies" sheetId="2" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>babies</t>
   </si>
   <si>
-    <t>babies_potential</t>
-  </si>
-  <si>
     <t>old_alloc_list</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>bb30</t>
+  </si>
+  <si>
+    <t>babies_service</t>
   </si>
 </sst>
 </file>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFF5F45-CFAD-4E61-9970-5F5BE534E7C0}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,18 +618,18 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -739,222 +739,222 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE173FA1-E983-499D-AB64-6CD8215CA3C5}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+    <sheetView zoomScale="103" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -985,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -994,22 +994,22 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1020,10 +1020,10 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1174,7 +1174,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -1503,7 +1503,7 @@
         <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Improvement] On terminology : room -> bed
</commit_message>
<xml_diff>
--- a/scenarios/exemple/input_exemple.xlsx
+++ b/scenarios/exemple/input_exemple.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS5997\src\neonat\scenarios\exemple\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C398C0-EBF0-43D7-B951-C2698F36A864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8218D47D-EDCD-42EC-BFFB-7474AE8B5C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="babies" sheetId="2" r:id="rId1"/>
-    <sheet name="rooms" sheetId="3" r:id="rId2"/>
+    <sheet name="beds" sheetId="3" r:id="rId2"/>
     <sheet name="services" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -62,15 +62,9 @@
     <t>r7</t>
   </si>
   <si>
-    <t>new_rooms_service</t>
-  </si>
-  <si>
     <t>out</t>
   </si>
   <si>
-    <t>old_rooms</t>
-  </si>
-  <si>
     <t>r8</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>r10</t>
   </si>
   <si>
-    <t>new_rooms</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -155,18 +146,9 @@
     <t>n30</t>
   </si>
   <si>
-    <t>old_rooms_service</t>
-  </si>
-  <si>
     <t>leave_hospital</t>
   </si>
   <si>
-    <t>rooms_capacities</t>
-  </si>
-  <si>
-    <t>all_rooms</t>
-  </si>
-  <si>
     <t>soins,neo</t>
   </si>
   <si>
@@ -267,6 +249,24 @@
   </si>
   <si>
     <t>babies_service</t>
+  </si>
+  <si>
+    <t>all_beds</t>
+  </si>
+  <si>
+    <t>new_beds</t>
+  </si>
+  <si>
+    <t>old_beds</t>
+  </si>
+  <si>
+    <t>new_beds_service</t>
+  </si>
+  <si>
+    <t>old_beds_service</t>
+  </si>
+  <si>
+    <t>beds_capacities</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFF5F45-CFAD-4E61-9970-5F5BE534E7C0}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+    <sheetView zoomScale="102" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -615,21 +615,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -706,255 +706,255 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE173FA1-E983-499D-AB64-6CD8215CA3C5}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,45 +985,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1031,7 +1031,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1045,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -1059,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -1073,7 +1073,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
@@ -1087,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -1101,7 +1101,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -1174,13 +1174,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
@@ -1194,13 +1194,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -1234,13 +1234,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -1314,13 +1314,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -1334,13 +1334,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -1394,13 +1394,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
@@ -1414,13 +1414,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -1454,13 +1454,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
@@ -1494,16 +1494,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
@@ -1514,13 +1514,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
@@ -1534,13 +1534,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
@@ -1554,13 +1554,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>